<commit_message>
cambios realizados en la clase Materia, ahora los prerequisitos se guardan como una lista de strings separados por comas o slashes.
</commit_message>
<xml_diff>
--- a/Data/Materias Mecatrónica.xlsx
+++ b/Data/Materias Mecatrónica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Desktop\App Pensum\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D1BE9D-4181-403F-A31E-EF1DB98F0D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF99B5D4-EDBD-42F7-BCC4-1DE63E2F17E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,10 +56,6 @@
     <t>Pendiente</t>
   </si>
   <si>
-    <t xml:space="preserve"> Créditos 
-Requisitos</t>
-  </si>
-  <si>
     <t>CÁTEDRA FARÍA</t>
   </si>
   <si>
@@ -219,9 +215,6 @@
     <t>REDES Y COMUNICACIONES INDUSTRIALES</t>
   </si>
   <si>
-    <t>168416, 168238</t>
-  </si>
-  <si>
     <t>APIE</t>
   </si>
   <si>
@@ -243,13 +236,19 @@
     <t>SEMINARIO MMI</t>
   </si>
   <si>
-    <t>168452, 168209</t>
-  </si>
-  <si>
     <t>FORMACIÓN CIUDADANA Y CULTURA DE LA PAZ</t>
   </si>
   <si>
     <t>TRABAJO DE GRADO</t>
+  </si>
+  <si>
+    <t>Creditos_Requisitos</t>
+  </si>
+  <si>
+    <t>168452/168209</t>
+  </si>
+  <si>
+    <t>168416/168238</t>
   </si>
 </sst>
 </file>
@@ -318,13 +317,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -633,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="132" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,7 +642,7 @@
     <col min="2" max="2" width="44.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="2" customWidth="1"/>
     <col min="7" max="7" width="12.140625" style="2" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
@@ -666,7 +665,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -677,7 +676,7 @@
         <v>153002</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -697,7 +696,7 @@
         <v>162274</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2">
         <v>1</v>
@@ -717,7 +716,7 @@
         <v>157400</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -737,7 +736,7 @@
         <v>164004</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2">
         <v>1</v>
@@ -757,7 +756,7 @@
         <v>162003</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -777,7 +776,7 @@
         <v>167389</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -797,7 +796,7 @@
         <v>168408</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
@@ -817,7 +816,7 @@
         <v>162275</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
@@ -840,7 +839,7 @@
         <v>157408</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="2">
         <v>2</v>
@@ -860,7 +859,7 @@
         <v>157401</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2">
         <v>2</v>
@@ -883,7 +882,7 @@
         <v>167344</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2">
         <v>2</v>
@@ -903,7 +902,7 @@
         <v>157405</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="2">
         <v>2</v>
@@ -923,7 +922,7 @@
         <v>168409</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2">
         <v>2</v>
@@ -943,7 +942,7 @@
         <v>168410</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="2">
         <v>2</v>
@@ -963,7 +962,7 @@
         <v>162276</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="2">
         <v>3</v>
@@ -986,7 +985,7 @@
         <v>157402</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2">
         <v>3</v>
@@ -1010,7 +1009,7 @@
         <v>157406</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="2">
         <v>3</v>
@@ -1033,7 +1032,7 @@
         <v>167105</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="2">
         <v>3</v>
@@ -1056,7 +1055,7 @@
         <v>150001</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2">
         <v>3</v>
@@ -1076,7 +1075,7 @@
         <v>167105</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="2">
         <v>3</v>
@@ -1096,7 +1095,7 @@
         <v>168411</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="2">
         <v>3</v>
@@ -1119,7 +1118,7 @@
         <v>157403</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="2">
         <v>4</v>
@@ -1142,7 +1141,7 @@
         <v>157407</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="2">
         <v>4</v>
@@ -1165,7 +1164,7 @@
         <v>167353</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="2">
         <v>4</v>
@@ -1188,7 +1187,7 @@
         <v>167106</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="2">
         <v>4</v>
@@ -1211,7 +1210,7 @@
         <v>150002</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="2">
         <v>4</v>
@@ -1231,7 +1230,7 @@
         <v>168281</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="2">
         <v>4</v>
@@ -1254,7 +1253,7 @@
         <v>168412</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="2">
         <v>4</v>
@@ -1277,7 +1276,7 @@
         <v>167356</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="2">
         <v>5</v>
@@ -1300,7 +1299,7 @@
         <v>167112</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="2">
         <v>5</v>
@@ -1323,7 +1322,7 @@
         <v>168117</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="2">
         <v>5</v>
@@ -1346,7 +1345,7 @@
         <v>168280</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="2">
         <v>5</v>
@@ -1369,7 +1368,7 @@
         <v>168413</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="2">
         <v>5</v>
@@ -1392,7 +1391,7 @@
         <v>168414</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="2">
         <v>5</v>
@@ -1415,7 +1414,7 @@
         <v>168203</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="2">
         <v>6</v>
@@ -1438,7 +1437,7 @@
         <v>168209</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="2">
         <v>6</v>
@@ -1461,7 +1460,7 @@
         <v>167107</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" s="2">
         <v>6</v>
@@ -1484,7 +1483,7 @@
         <v>164010</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" s="2">
         <v>6</v>
@@ -1504,7 +1503,7 @@
         <v>168110</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" s="2">
         <v>6</v>
@@ -1527,7 +1526,7 @@
         <v>168452</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="2">
         <v>6</v>
@@ -1550,7 +1549,7 @@
         <v>168212</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="2">
         <v>7</v>
@@ -1570,7 +1569,7 @@
         <v>168238</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="2">
         <v>7</v>
@@ -1590,7 +1589,7 @@
         <v>168265</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" s="2">
         <v>7</v>
@@ -1613,7 +1612,7 @@
         <v>168416</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" s="2">
         <v>7</v>
@@ -1633,7 +1632,7 @@
         <v>168415</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="2">
         <v>7</v>
@@ -1656,7 +1655,7 @@
         <v>168428</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" s="2">
         <v>7</v>
@@ -1679,7 +1678,7 @@
         <v>171342</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="2">
         <v>8</v>
@@ -1699,7 +1698,7 @@
         <v>168419</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="2">
         <v>8</v>
@@ -1719,7 +1718,7 @@
         <v>168213</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" s="2">
         <v>8</v>
@@ -1739,7 +1738,7 @@
         <v>168266</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" s="2">
         <v>8</v>
@@ -1762,7 +1761,7 @@
         <v>168417</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C52" s="2">
         <v>8</v>
@@ -1771,7 +1770,7 @@
         <v>3</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="F52" s="2">
         <v>0</v>
@@ -1785,7 +1784,7 @@
         <v>168418</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C53" s="2">
         <v>8</v>
@@ -1808,7 +1807,7 @@
         <v>167336</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C54" s="2">
         <v>8</v>
@@ -1828,7 +1827,7 @@
         <v>168423</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C55" s="2">
         <v>9</v>
@@ -1848,7 +1847,7 @@
         <v>168214</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C56" s="2">
         <v>9</v>
@@ -1868,7 +1867,7 @@
         <v>168215</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C57" s="2">
         <v>9</v>
@@ -1888,7 +1887,7 @@
         <v>168420</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C58" s="2">
         <v>9</v>
@@ -1911,7 +1910,7 @@
         <v>168424</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C59" s="2">
         <v>9</v>
@@ -1934,7 +1933,7 @@
         <v>168422</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C60" s="2">
         <v>9</v>
@@ -1943,7 +1942,7 @@
         <v>3</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F60" s="2">
         <v>0</v>
@@ -1957,7 +1956,7 @@
         <v>168421</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C61" s="2">
         <v>9</v>
@@ -1977,7 +1976,7 @@
         <v>164335</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C62" s="2">
         <v>10</v>
@@ -1997,7 +1996,7 @@
         <v>168425</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C63" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
Integra lógica dinámica de aprobación y seguimiento de pensum
Implementa clases para representar materias y el plan de estudios, permitiendo el cálculo dinámico de requisitos previos y créditos. Actualiza la interfaz para cargar datos reales, mostrar el progreso del crédito y reflejar los estados de las materias con códigos de colores. Mejora la experiencia del usuario al permitir la aprobación interactiva de materias, actualizar materias dependientes y brindar comentarios sobre la graduación.
</commit_message>
<xml_diff>
--- a/Data/Materias Mecatrónica.xlsx
+++ b/Data/Materias Mecatrónica.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Desktop\App Pensum\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C894C9B-9B1E-4B91-8738-27F835CF3E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82685F2C-C631-4CD5-83A5-CACAFDC0BAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="825" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="74">
   <si>
     <t>Código</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>157401</t>
+  </si>
+  <si>
+    <t>168108</t>
   </si>
 </sst>
 </file>
@@ -635,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="132" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,8 +1077,8 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>167105</v>
+      <c r="A21" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>26</v>
@@ -1241,8 +1244,8 @@
       <c r="D28" s="2">
         <v>2</v>
       </c>
-      <c r="E28" s="2">
-        <v>167105</v>
+      <c r="E28" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="F28" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
Mejora la interfaz gráfica y actualiza la lógica de aprobación de materias, incluyendo un nuevo mensaje de advertencia para los prerrequisitos.
</commit_message>
<xml_diff>
--- a/Data/Materias Mecatrónica.xlsx
+++ b/Data/Materias Mecatrónica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Desktop\App Pensum\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82685F2C-C631-4CD5-83A5-CACAFDC0BAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAEEA2D-71B0-4182-92CA-9FFD62DA29EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="825" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="132" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,16 +679,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>153002</v>
+        <v>171342</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C2" s="2">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
         <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>2</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -699,13 +699,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>162274</v>
+        <v>157408</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2">
         <v>2</v>
@@ -719,19 +719,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>157400</v>
+        <v>168423</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="2">
         <v>9</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
       <c r="D4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" s="2">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>6</v>
@@ -739,19 +739,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>164004</v>
+        <v>168416</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>6</v>
@@ -759,16 +759,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>162003</v>
+        <v>168417</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="F6" s="2">
         <v>0</v>
@@ -779,16 +782,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>167389</v>
+        <v>168420</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E7" s="2">
+        <v>168417</v>
       </c>
       <c r="F7" s="2">
         <v>0</v>
@@ -799,16 +805,16 @@
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>168408</v>
+        <v>157400</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>
       </c>
       <c r="D8" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
@@ -818,20 +824,20 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>162275</v>
+      <c r="A9" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2">
         <v>2</v>
       </c>
       <c r="D9" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" s="2">
-        <v>162274</v>
+        <v>157400</v>
       </c>
       <c r="F9" s="2">
         <v>0</v>
@@ -842,16 +848,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>157408</v>
+        <v>157402</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D10" s="2">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E10" s="2">
+        <v>157401</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -861,20 +870,17 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>72</v>
+      <c r="A11" s="2">
+        <v>153002</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>3</v>
-      </c>
-      <c r="E11" s="2">
-        <v>157400</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -885,16 +891,19 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>167344</v>
+        <v>167105</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C12" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="2">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E12" s="2">
+        <v>157401</v>
       </c>
       <c r="F12" s="2">
         <v>0</v>
@@ -905,16 +914,19 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>157405</v>
+        <v>167106</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" s="2">
         <v>3</v>
+      </c>
+      <c r="E13" s="2">
+        <v>167105</v>
       </c>
       <c r="F13" s="2">
         <v>0</v>
@@ -925,16 +937,19 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>168409</v>
+        <v>168203</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C14" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>168413</v>
       </c>
       <c r="F14" s="2">
         <v>0</v>
@@ -945,16 +960,19 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>168410</v>
+        <v>168415</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E15" s="2">
+        <v>168203</v>
       </c>
       <c r="F15" s="2">
         <v>0</v>
@@ -965,19 +983,19 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>162276</v>
+        <v>168428</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C16" s="2">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D16" s="2">
         <v>2</v>
       </c>
       <c r="E16" s="2">
-        <v>162275</v>
+        <v>168203</v>
       </c>
       <c r="F16" s="2">
         <v>0</v>
@@ -988,19 +1006,19 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>157402</v>
+        <v>168418</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="C17" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D17" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2">
-        <v>157401</v>
+        <v>168428</v>
       </c>
       <c r="F17" s="2">
         <v>0</v>
@@ -1012,19 +1030,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>157406</v>
+        <v>168424</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>23</v>
+        <v>64</v>
       </c>
       <c r="C18" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2">
-        <v>157405</v>
+        <v>168110</v>
       </c>
       <c r="F18" s="2">
         <v>0</v>
@@ -1035,19 +1053,16 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>167105</v>
+        <v>168409</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C19" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2">
-        <v>3</v>
-      </c>
-      <c r="E19" s="2">
-        <v>157401</v>
+        <v>2</v>
       </c>
       <c r="F19" s="2">
         <v>0</v>
@@ -1058,16 +1073,19 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>150001</v>
+        <v>168280</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C20" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D20" s="2">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>168281</v>
       </c>
       <c r="F20" s="2">
         <v>0</v>
@@ -1077,18 +1095,21 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>73</v>
+      <c r="A21" s="2">
+        <v>168209</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C21" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D21" s="2">
         <v>2</v>
       </c>
+      <c r="E21" s="2">
+        <v>168280</v>
+      </c>
       <c r="F21" s="2">
         <v>0</v>
       </c>
@@ -1096,21 +1117,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>168411</v>
+        <v>168422</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C22" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D22" s="2">
-        <v>2</v>
-      </c>
-      <c r="E22" s="2">
-        <v>167344</v>
+        <v>3</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="F22" s="2">
         <v>0</v>
@@ -1144,19 +1165,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>157407</v>
+        <v>164004</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C24" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2">
-        <v>3</v>
-      </c>
-      <c r="E24" s="2">
-        <v>157406</v>
+        <v>2</v>
       </c>
       <c r="F24" s="2">
         <v>0</v>
@@ -1167,22 +1185,19 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>167353</v>
+        <v>168212</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C25" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D25" s="2">
-        <v>3</v>
-      </c>
-      <c r="E25" s="2">
-        <v>167105</v>
+        <v>2</v>
       </c>
       <c r="F25" s="2">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>6</v>
@@ -1190,22 +1205,19 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>167106</v>
+        <v>168213</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C26" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D26" s="2">
-        <v>3</v>
-      </c>
-      <c r="E26" s="2">
-        <v>167105</v>
+        <v>2</v>
       </c>
       <c r="F26" s="2">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>6</v>
@@ -1213,19 +1225,19 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>150002</v>
+        <v>168214</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>32</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D27" s="2">
         <v>2</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>6</v>
@@ -1233,22 +1245,19 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>168281</v>
+        <v>168215</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>33</v>
+        <v>62</v>
       </c>
       <c r="C28" s="2">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>73</v>
-      </c>
       <c r="F28" s="2">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>6</v>
@@ -1256,19 +1265,16 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>168412</v>
+        <v>150001</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C29" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
-      </c>
-      <c r="E29" s="2">
-        <v>168411</v>
       </c>
       <c r="F29" s="2">
         <v>0</v>
@@ -1279,19 +1285,16 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>167356</v>
+        <v>150002</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C30" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2">
-        <v>3</v>
-      </c>
-      <c r="E30" s="2">
-        <v>167353</v>
+        <v>2</v>
       </c>
       <c r="F30" s="2">
         <v>0</v>
@@ -1302,19 +1305,19 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>167112</v>
+        <v>157406</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C31" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D31" s="2">
         <v>3</v>
       </c>
       <c r="E31" s="2">
-        <v>167106</v>
+        <v>157405</v>
       </c>
       <c r="F31" s="2">
         <v>0</v>
@@ -1325,19 +1328,19 @@
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>168117</v>
+        <v>167353</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C32" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D32" s="2">
         <v>3</v>
       </c>
       <c r="E32" s="2">
-        <v>157403</v>
+        <v>167105</v>
       </c>
       <c r="F32" s="2">
         <v>0</v>
@@ -1348,10 +1351,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>168280</v>
+        <v>167356</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2">
         <v>5</v>
@@ -1360,7 +1363,7 @@
         <v>3</v>
       </c>
       <c r="E33" s="2">
-        <v>168281</v>
+        <v>167353</v>
       </c>
       <c r="F33" s="2">
         <v>0</v>
@@ -1369,21 +1372,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
-        <v>168413</v>
+        <v>167107</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C34" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D34" s="2">
         <v>3</v>
       </c>
       <c r="E34" s="2">
-        <v>157403</v>
+        <v>167356</v>
       </c>
       <c r="F34" s="2">
         <v>0</v>
@@ -1394,19 +1397,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
-        <v>168414</v>
+        <v>164010</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C35" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D35" s="2">
         <v>2</v>
-      </c>
-      <c r="E35" s="2">
-        <v>168412</v>
       </c>
       <c r="F35" s="2">
         <v>0</v>
@@ -1417,19 +1417,16 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>168203</v>
+        <v>164335</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="C36" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D36" s="2">
-        <v>4</v>
-      </c>
-      <c r="E36" s="2">
-        <v>168413</v>
+        <v>1</v>
       </c>
       <c r="F36" s="2">
         <v>0</v>
@@ -1440,20 +1437,17 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>168209</v>
+        <v>167344</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C37" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D37" s="2">
         <v>2</v>
       </c>
-      <c r="E37" s="2">
-        <v>168280</v>
-      </c>
       <c r="F37" s="2">
         <v>0</v>
       </c>
@@ -1461,21 +1455,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>167107</v>
+        <v>168411</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C38" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D38" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E38" s="2">
-        <v>167356</v>
+        <v>167344</v>
       </c>
       <c r="F38" s="2">
         <v>0</v>
@@ -1486,13 +1480,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>164010</v>
+        <v>162003</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="C39" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D39" s="2">
         <v>2</v>
@@ -1506,19 +1500,16 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>168110</v>
+        <v>167389</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="C40" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D40" s="2">
-        <v>3</v>
-      </c>
-      <c r="E40" s="2">
-        <v>168281</v>
+        <v>1</v>
       </c>
       <c r="F40" s="2">
         <v>0</v>
@@ -1529,19 +1520,16 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>168452</v>
+        <v>162274</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C41" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D41" s="2">
-        <v>3</v>
-      </c>
-      <c r="E41" s="2">
-        <v>168414</v>
+        <v>2</v>
       </c>
       <c r="F41" s="2">
         <v>0</v>
@@ -1552,19 +1540,22 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>168212</v>
+        <v>162275</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>47</v>
+        <v>14</v>
       </c>
       <c r="C42" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D42" s="2">
         <v>2</v>
       </c>
+      <c r="E42" s="2">
+        <v>162274</v>
+      </c>
       <c r="F42" s="2">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>6</v>
@@ -1572,19 +1563,22 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>168238</v>
+        <v>162276</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="C43" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D43" s="2">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E43" s="2">
+        <v>162275</v>
       </c>
       <c r="F43" s="2">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>6</v>
@@ -1592,22 +1586,19 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>168265</v>
+        <v>168238</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C44" s="2">
         <v>7</v>
       </c>
       <c r="D44" s="2">
-        <v>4</v>
-      </c>
-      <c r="E44" s="2">
-        <v>168452</v>
+        <v>3</v>
       </c>
       <c r="F44" s="2">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>6</v>
@@ -1615,19 +1606,19 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>168416</v>
+        <v>168408</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C45" s="2">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D45" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F45" s="2">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>6</v>
@@ -1635,19 +1626,19 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
-        <v>168415</v>
+        <v>167112</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C46" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D46" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E46" s="2">
-        <v>168203</v>
+        <v>167106</v>
       </c>
       <c r="F46" s="2">
         <v>0</v>
@@ -1658,19 +1649,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
-        <v>168428</v>
+        <v>157405</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="C47" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D47" s="2">
-        <v>2</v>
-      </c>
-      <c r="E47" s="2">
-        <v>168203</v>
+        <v>3</v>
       </c>
       <c r="F47" s="2">
         <v>0</v>
@@ -1680,17 +1668,17 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>171342</v>
+      <c r="A48" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="C48" s="2">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D48" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F48" s="2">
         <v>0</v>
@@ -1701,16 +1689,19 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
-        <v>168419</v>
+        <v>168281</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C49" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D49" s="2">
         <v>2</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="F49" s="2">
         <v>0</v>
@@ -1721,39 +1712,42 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
-        <v>168213</v>
+        <v>168452</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C50" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D50" s="2">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E50" s="2">
+        <v>168414</v>
       </c>
       <c r="F50" s="2">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
-        <v>168266</v>
+        <v>168413</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C51" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D51" s="2">
         <v>3</v>
       </c>
       <c r="E51" s="2">
-        <v>168265</v>
+        <v>157403</v>
       </c>
       <c r="F51" s="2">
         <v>0</v>
@@ -1764,19 +1758,19 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
-        <v>168417</v>
+        <v>157407</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C52" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D52" s="2">
         <v>3</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>71</v>
+      <c r="E52" s="2">
+        <v>157406</v>
       </c>
       <c r="F52" s="2">
         <v>0</v>
@@ -1787,10 +1781,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
-        <v>168418</v>
+        <v>168419</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C53" s="2">
         <v>8</v>
@@ -1798,9 +1792,6 @@
       <c r="D53" s="2">
         <v>2</v>
       </c>
-      <c r="E53" s="2">
-        <v>168428</v>
-      </c>
       <c r="F53" s="2">
         <v>0</v>
       </c>
@@ -1810,19 +1801,22 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
-        <v>167336</v>
+        <v>168110</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C54" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D54" s="2">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="E54" s="2">
+        <v>168281</v>
       </c>
       <c r="F54" s="2">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>6</v>
@@ -1830,19 +1824,22 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
-        <v>168423</v>
+        <v>168412</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C55" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D55" s="2">
         <v>2</v>
       </c>
+      <c r="E55" s="2">
+        <v>168411</v>
+      </c>
       <c r="F55" s="2">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>6</v>
@@ -1850,19 +1847,22 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
-        <v>168214</v>
+        <v>168414</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C56" s="2">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D56" s="2">
         <v>2</v>
       </c>
+      <c r="E56" s="2">
+        <v>168412</v>
+      </c>
       <c r="F56" s="2">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>6</v>
@@ -1870,19 +1870,19 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
-        <v>168215</v>
+        <v>167336</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C57" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D57" s="2">
         <v>2</v>
       </c>
       <c r="F57" s="2">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>6</v>
@@ -1890,19 +1890,19 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
-        <v>168420</v>
+        <v>168265</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="C58" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D58" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E58" s="2">
-        <v>168417</v>
+        <v>168452</v>
       </c>
       <c r="F58" s="2">
         <v>0</v>
@@ -1913,19 +1913,19 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
-        <v>168424</v>
+        <v>168266</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C59" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D59" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E59" s="2">
-        <v>168110</v>
+        <v>168265</v>
       </c>
       <c r="F59" s="2">
         <v>0</v>
@@ -1936,22 +1936,19 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
-        <v>168422</v>
+        <v>168421</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C60" s="2">
         <v>9</v>
       </c>
       <c r="D60" s="2">
-        <v>3</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="F60" s="2">
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>6</v>
@@ -1959,19 +1956,19 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
-        <v>168421</v>
+        <v>168410</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="C61" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D61" s="2">
         <v>2</v>
       </c>
       <c r="F61" s="2">
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>6</v>
@@ -1979,16 +1976,19 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
-        <v>164335</v>
+        <v>168117</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="C62" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D62" s="2">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="E62" s="2">
+        <v>157403</v>
       </c>
       <c r="F62" s="2">
         <v>0</v>
@@ -2018,6 +2018,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G63">
+    <sortCondition ref="B1:B63"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>